<commit_message>
Purified code - now with RuboCop
</commit_message>
<xml_diff>
--- a/tests/test1.xlsx
+++ b/tests/test1.xlsx
@@ -396,39 +396,27 @@
         <v>a</v>
       </c>
       <c r="C2" s="0" t="str">
-        <v>Число для примеру</v>
+        <v>тестовые данные</v>
       </c>
       <c r="D2" s="0" t="str">
-        <v>integer, int</v>
+        <v/>
       </c>
       <c r="E2" s="0" t="str">
-        <v>Простая переменная</v>
+        <v/>
       </c>
       <c r="F2" s="0" t="str">
-        <v>[0 - 100]</v>
+        <v/>
       </c>
       <c r="G2" s="0" t="str">
-        <v>Число</v>
+        <v xml:space="preserve">[5..600]  </v>
       </c>
     </row>
-    <row r="3" spans="1:6" customFormat="false">
+    <row r="3" spans="1:2" customFormat="false">
       <c r="A3" s="0" t="str">
         <v/>
       </c>
       <c r="B3" s="0" t="str">
-        <v/>
-      </c>
-      <c r="C3" s="0" t="str">
-        <v>HelloWorld</v>
-      </c>
-      <c r="D3" s="0" t="str">
-        <v/>
-      </c>
-      <c r="E3" s="0" t="str">
-        <v/>
-      </c>
-      <c r="F3" s="0" t="str">
-        <v/>
+        <v xml:space="preserve">Не найден  </v>
       </c>
     </row>
   </sheetData>

</xml_diff>